<commit_message>
Evaluation document for cognitive walk through
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/cognitive_walkthrough/phase_3.xlsx
+++ b/Project supporting Artifacts/Evaluation/cognitive_walkthrough/phase_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanmccrossan/group_project/TUD-Group-Project/Project supporting Artifacts/Evaluation/cognitive_walkthrough/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13196DE3-29AD-BA47-AF5F-BEDA28B8B78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E5E63F-2127-3245-86EE-3469FE4104D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{9E940733-D15D-444C-A26B-A567DC9AD4B9}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="15">
-  <si>
-    <t>Task 1 - Upload the data</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="18">
   <si>
     <t>User:</t>
   </si>
@@ -59,21 +56,6 @@
     <t xml:space="preserve">Feedback from user: </t>
   </si>
   <si>
-    <t>Task 1 - Which column has the most missing values?</t>
-  </si>
-  <si>
-    <t>Task 3 - Check the outliers in your data</t>
-  </si>
-  <si>
-    <t>Task 4 - Determine the quality of your data</t>
-  </si>
-  <si>
-    <t>Task 5 - Clean your data</t>
-  </si>
-  <si>
-    <t>Task 6 - Export the data</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -81,6 +63,33 @@
   </si>
   <si>
     <t>User 4</t>
+  </si>
+  <si>
+    <t>Task 1 - Register and Login</t>
+  </si>
+  <si>
+    <t>Task 3 - Navigate to data preview page and determine whether your data uploaded correctly</t>
+  </si>
+  <si>
+    <t>Task 2 - Data Upload</t>
+  </si>
+  <si>
+    <t>Task 4 - Determine which column has the most missing values</t>
+  </si>
+  <si>
+    <t>Task 5 - Determine the quality of your data</t>
+  </si>
+  <si>
+    <t>Task 6 - Determine if there are any correlations within the data</t>
+  </si>
+  <si>
+    <t>Task 7 - Remove duplicates</t>
+  </si>
+  <si>
+    <t>Task 8 - Clean your data based on the information you have.</t>
+  </si>
+  <si>
+    <t>Task 9 - Export the data</t>
   </si>
 </sst>
 </file>
@@ -462,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233B0C84-AB2A-1742-9CD1-4F33E13FF503}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,7 +487,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -487,75 +496,75 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -564,75 +573,82 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -641,75 +657,75 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -718,75 +734,75 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -795,75 +811,75 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="D26" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -872,80 +888,314 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="D32" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A49:E49"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A13:E13"/>
     <mergeCell ref="A19:E19"/>
     <mergeCell ref="A25:E25"/>
     <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A37:E37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>